<commit_message>
final version for prelim
</commit_message>
<xml_diff>
--- a/adsphd-master/chapters/aquacrop/image/All figures.xlsx
+++ b/adsphd-master/chapters/aquacrop/image/All figures.xlsx
@@ -68,7 +68,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>331200</xdr:colOff>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>117029</xdr:rowOff>
     </xdr:to>
@@ -81,7 +81,7 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect t="1055"/>
+        <a:srcRect t="1055" r="9160"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -89,7 +89,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2160000" cy="2022029"/>
+          <a:ext cx="1962150" cy="2022029"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>